<commit_message>
feature: zhong xin scan complete
</commit_message>
<xml_diff>
--- a/equipment_cyg/product/zhong_xin_scan/zhong_xin_scan_manual.xlsx
+++ b/equipment_cyg/product/zhong_xin_scan/zhong_xin_scan_manual.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="504" activeTab="6"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="504" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="secs指令" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">secs指令!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">plc!$D$1:$D$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">plc!$D$1:$D$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="307">
   <si>
     <t>direction</t>
   </si>
@@ -287,6 +287,12 @@
     <t>出站</t>
   </si>
   <si>
+    <t>success_count</t>
+  </si>
+  <si>
+    <t>OK的产品数量</t>
+  </si>
+  <si>
     <t>track_out_product_sns</t>
   </si>
   <si>
@@ -302,6 +308,24 @@
     <t>出站产品状态</t>
   </si>
   <si>
+    <t>lot_end</t>
+  </si>
+  <si>
+    <t>工单结束</t>
+  </si>
+  <si>
+    <t>lot_name</t>
+  </si>
+  <si>
+    <t>本次工单名称</t>
+  </si>
+  <si>
+    <t>lot_number</t>
+  </si>
+  <si>
+    <t>本次工单要求生产OK数量</t>
+  </si>
+  <si>
     <t>VID</t>
   </si>
   <si>
@@ -353,60 +377,60 @@
     <t>values</t>
   </si>
   <si>
-    <t>0：offline，设备被离线
-1:Online Local，本地在线
-2:Online Remote，远程模式在线</t>
-  </si>
-  <si>
-    <t>1:Manual,手动模式
-2:Auto，自动模式停止状态
-3:AutoRun,自动模式启动状态
-4:Alarm
-5:Schedule down
-6:Engineer</t>
+    <t>BOOL</t>
+  </si>
+  <si>
+    <t>0：设备离线
+1：Online Local
+2：Online Remote</t>
+  </si>
+  <si>
+    <t>1:Manual
+2:Auto，自动模式下停止
+3:AutoRun，自动模式下运行
+4:初始化</t>
   </si>
   <si>
     <t>data_id</t>
   </si>
   <si>
-    <t>1：切换成功
-3：设备machine_state不处于手动状态，不允许切换
-4：设备控制状态处于Online Local状态,不允许切换,控制状态处于Online Remote才允许切换</t>
-  </si>
-  <si>
-    <t>0：ng，1：ok，2：有mark点</t>
+    <t>1：OK
+3：当前machine_state不是手动Manual状态
+4：当前设备控制状态不是Online Remote</t>
+  </si>
+  <si>
+    <t>1：OK
+2：NG
+3：有mark点</t>
   </si>
   <si>
     <t>upload_recipe_id</t>
   </si>
   <si>
-    <t>上传的配方id</t>
+    <t>上传配方id</t>
   </si>
   <si>
     <t>upload_recipe_name</t>
   </si>
   <si>
-    <t>上传的配方name</t>
+    <t>上传配方name</t>
   </si>
   <si>
     <t>pp_select_recipe_id</t>
   </si>
   <si>
-    <t>切换的配方id</t>
+    <t>切换配方id</t>
   </si>
   <si>
     <t>pp_select_recipe_name</t>
   </si>
   <si>
-    <t>切换的配方name</t>
+    <t>切换配方name</t>
   </si>
   <si>
     <t>track_in_reply_flag</t>
   </si>
   <si>
-    <t>BOOL</t>
-  </si>
-  <si>
     <t>进站是否回复</t>
   </si>
   <si>
@@ -419,9 +443,27 @@
     <t>recipe_id_name</t>
   </si>
   <si>
-    <t>1：切换成功
-3：设备machine_state不处于1手动状态，不允许切换
-4：设备控制状态处于Online Local状态,不允许切换,控制状态处于Online Remote才允许切换</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">切换配方
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>只有当前502:currnet_machine_state运行状态是1:手动模式才能切换配方</t>
+    </r>
   </si>
   <si>
     <t>track_in_reply</t>
@@ -433,6 +475,15 @@
     <t>1:ok,2:ng</t>
   </si>
   <si>
+    <t>new_lot</t>
+  </si>
+  <si>
+    <t>lot_name，lot_number</t>
+  </si>
+  <si>
+    <t>开工单，lot_number表示要生产的数量</t>
+  </si>
+  <si>
     <t>标签</t>
   </si>
   <si>
@@ -536,6 +587,15 @@
   </si>
   <si>
     <t>配方上传响应</t>
+  </si>
+  <si>
+    <t>是否可以进站</t>
+  </si>
+  <si>
+    <t>Application.UN0_MES.xToPlcAllowInletNotice</t>
+  </si>
+  <si>
+    <t>EAP管控托盘是否可以进站</t>
   </si>
   <si>
     <t>Application.UN0_MES.sToPCVencileCode</t>
@@ -1016,7 +1076,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1289,6 +1349,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="42">
@@ -2769,7 +2836,7 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -3051,27 +3118,27 @@
   <sheetData>
     <row r="1" ht="21.75" spans="4:4">
       <c r="D1" s="2" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" ht="16.5" spans="4:9">
       <c r="D2" s="3" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="4:9">
@@ -3079,7 +3146,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
@@ -3088,10 +3155,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="4:9">
@@ -3100,7 +3167,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="8" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="I4" s="41"/>
     </row>
@@ -3110,7 +3177,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="8" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="I5" s="41"/>
     </row>
@@ -3120,7 +3187,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="I6" s="41"/>
     </row>
@@ -3130,7 +3197,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="8" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="I7" s="42"/>
     </row>
@@ -3139,7 +3206,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
@@ -3148,16 +3215,16 @@
         <v>2</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="K8" s="43" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="M8" s="44"/>
     </row>
@@ -3167,17 +3234,17 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="8" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="I9" s="41"/>
       <c r="K9" s="14">
         <v>1</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="M9" s="45" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" ht="16.5" spans="4:13">
@@ -3186,13 +3253,13 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="8" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="I10" s="41"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="45" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" ht="16.5" spans="4:13">
@@ -3201,13 +3268,13 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="8" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="I11" s="42"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="45" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" ht="16.5" spans="4:13">
@@ -3215,7 +3282,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="F12" s="12">
         <v>3</v>
@@ -3224,15 +3291,15 @@
         <v>3</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="45" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" ht="16.5" spans="4:13">
@@ -3240,7 +3307,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="F13" s="15">
         <v>4</v>
@@ -3249,15 +3316,15 @@
         <v>4</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="46" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" ht="16.5" spans="4:13">
@@ -3268,19 +3335,19 @@
         <v>5</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="K14" s="14">
         <v>2</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="M14" s="45" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" ht="16.5" spans="4:13">
@@ -3288,7 +3355,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="F15" s="15">
         <v>5</v>
@@ -3297,15 +3364,15 @@
         <v>4</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="45" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" ht="16.5" spans="4:13">
@@ -3316,15 +3383,15 @@
         <v>5</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="45" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" ht="16.5" spans="4:13">
@@ -3335,15 +3402,15 @@
         <v>6</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="46" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" ht="16.5" spans="4:13">
@@ -3351,7 +3418,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="F18" s="15">
         <v>6</v>
@@ -3360,19 +3427,19 @@
         <v>4</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="K18" s="11">
         <v>3</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="M18" s="46" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" ht="16.5" spans="4:13">
@@ -3380,7 +3447,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -3390,10 +3457,10 @@
         <v>4</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="M19" s="46" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" ht="16.5" spans="4:9">
@@ -3401,7 +3468,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="F20" s="15">
         <v>8</v>
@@ -3410,10 +3477,10 @@
         <v>8</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" ht="16.5" spans="4:9">
@@ -3421,7 +3488,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -3433,7 +3500,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="F22" s="16">
         <v>10</v>
@@ -3442,10 +3509,10 @@
         <v>10</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" ht="16.5" spans="4:9">
@@ -3472,16 +3539,16 @@
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
       <c r="K25" s="47" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="L25" s="48" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="M25" s="48" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="N25" s="48" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" ht="32.25" spans="4:14">
@@ -3492,40 +3559,40 @@
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
       <c r="K26" s="49" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="L26" s="50" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="M26" s="50"/>
       <c r="N26" s="50" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" ht="16.5" spans="4:14">
       <c r="D27" s="11"/>
       <c r="E27" s="16" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
       <c r="K27" s="49" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="L27" s="50" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="M27" s="50"/>
       <c r="N27" s="50" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" ht="16.5" spans="4:9">
       <c r="D28" s="23"/>
       <c r="E28" s="16" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -3535,45 +3602,45 @@
     <row r="37" ht="14.25"/>
     <row r="38" ht="16.5" spans="4:10">
       <c r="D38" s="24" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="G38" s="25" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="I38" s="51" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="J38" s="52" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" ht="16.5" spans="4:10">
       <c r="D39" s="27" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="H39" s="11">
         <v>1</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="J39" s="12">
         <v>2</v>
@@ -3583,14 +3650,14 @@
       <c r="D40" s="30"/>
       <c r="E40" s="31"/>
       <c r="F40" s="29" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="11">
         <v>2</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="J40" s="12">
         <v>2</v>
@@ -3600,7 +3667,7 @@
       <c r="D41" s="30"/>
       <c r="E41" s="31"/>
       <c r="F41" s="32" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="G41" s="31"/>
     </row>
@@ -3608,7 +3675,7 @@
       <c r="D42" s="30"/>
       <c r="E42" s="31"/>
       <c r="F42" s="33" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="G42" s="31"/>
     </row>
@@ -3616,7 +3683,7 @@
       <c r="D43" s="30"/>
       <c r="E43" s="31"/>
       <c r="F43" s="33" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="G43" s="31"/>
     </row>
@@ -3624,7 +3691,7 @@
       <c r="D44" s="30"/>
       <c r="E44" s="31"/>
       <c r="F44" s="33" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="G44" s="31"/>
     </row>
@@ -3632,7 +3699,7 @@
       <c r="D45" s="30"/>
       <c r="E45" s="31"/>
       <c r="F45" s="33" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="G45" s="31"/>
     </row>
@@ -3640,7 +3707,7 @@
       <c r="D46" s="30"/>
       <c r="E46" s="31"/>
       <c r="F46" s="33" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="G46" s="31"/>
     </row>
@@ -3648,7 +3715,7 @@
       <c r="D47" s="30"/>
       <c r="E47" s="31"/>
       <c r="F47" s="33" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="G47" s="31"/>
     </row>
@@ -3656,7 +3723,7 @@
       <c r="D48" s="30"/>
       <c r="E48" s="31"/>
       <c r="F48" s="33" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="G48" s="31"/>
     </row>
@@ -3664,7 +3731,7 @@
       <c r="D49" s="30"/>
       <c r="E49" s="31"/>
       <c r="F49" s="33" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="G49" s="31"/>
     </row>
@@ -3672,7 +3739,7 @@
       <c r="D50" s="30"/>
       <c r="E50" s="31"/>
       <c r="F50" s="33" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="G50" s="31"/>
     </row>
@@ -3680,7 +3747,7 @@
       <c r="D51" s="30"/>
       <c r="E51" s="31"/>
       <c r="F51" s="33" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="G51" s="31"/>
     </row>
@@ -3688,23 +3755,23 @@
       <c r="D52" s="34"/>
       <c r="E52" s="35"/>
       <c r="F52" s="36" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="G52" s="35"/>
     </row>
     <row r="53" ht="21" spans="4:4">
       <c r="D53" s="37" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" ht="15.75" spans="4:4">
       <c r="D54" s="38" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" ht="15.75" spans="4:4">
       <c r="D55" s="39" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -3749,12 +3816,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -3946,7 +4013,7 @@
       <c r="C8" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="91">
+      <c r="D8" s="104">
         <v>5</v>
       </c>
       <c r="E8" s="91">
@@ -3966,48 +4033,136 @@
       <c r="A9" s="91"/>
       <c r="B9" s="89"/>
       <c r="C9" s="90"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="91">
-        <v>604</v>
+      <c r="D9" s="108"/>
+      <c r="E9" s="89">
+        <v>504</v>
       </c>
       <c r="F9" s="89" t="s">
         <v>78</v>
       </c>
       <c r="G9" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="89" t="s">
         <v>79</v>
-      </c>
-      <c r="H9" s="89" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" s="99" customFormat="1" ht="18.75" spans="1:8">
       <c r="A10" s="91"/>
       <c r="B10" s="89"/>
       <c r="C10" s="90"/>
-      <c r="D10" s="91"/>
+      <c r="D10" s="91">
+        <v>6</v>
+      </c>
       <c r="E10" s="91">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F10" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="89" t="s">
         <v>81</v>
-      </c>
-      <c r="G10" s="89" t="s">
-        <v>79</v>
       </c>
       <c r="H10" s="89" t="s">
         <v>82</v>
       </c>
     </row>
+    <row r="11" s="99" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A11" s="91"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91">
+        <v>7</v>
+      </c>
+      <c r="E11" s="91">
+        <v>605</v>
+      </c>
+      <c r="F11" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="89" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="89" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" s="99" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A12" s="91">
+        <v>1006</v>
+      </c>
+      <c r="B12" s="89" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="91">
+        <v>8</v>
+      </c>
+      <c r="E12" s="89">
+        <v>504</v>
+      </c>
+      <c r="F12" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="89" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" s="99" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A13" s="91"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="89">
+        <v>505</v>
+      </c>
+      <c r="F13" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" s="99" customFormat="1" ht="18.75" spans="1:8">
+      <c r="A14" s="91"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="89">
+        <v>506</v>
+      </c>
+      <c r="F14" s="89" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="89" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A14"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C14"/>
     <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -4033,13 +4188,13 @@
   <sheetData>
     <row r="1" ht="16.5" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" ht="16.5" spans="1:3">
@@ -4047,10 +4202,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="96" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:4">
@@ -4058,13 +4213,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="96" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C3" s="97" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D3" s="98" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:4">
@@ -4072,10 +4227,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="96" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D4" s="98"/>
     </row>
@@ -4084,10 +4239,10 @@
         <v>100</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D5" s="98"/>
     </row>
@@ -4096,10 +4251,10 @@
         <v>200</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D6" s="98"/>
     </row>
@@ -4115,46 +4270,46 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelRow="3" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="9.13333333333333" style="92" customWidth="1"/>
     <col min="2" max="2" width="41" style="92" customWidth="1"/>
     <col min="3" max="3" width="21.3833333333333" style="92" customWidth="1"/>
     <col min="4" max="4" width="11.5333333333333" style="92" customWidth="1"/>
-    <col min="5" max="5" width="25.1333333333333" style="92" customWidth="1"/>
+    <col min="5" max="5" width="29.875" style="92" customWidth="1"/>
     <col min="6" max="6" width="36" style="92" customWidth="1"/>
     <col min="7" max="16384" width="9" style="92"/>
   </cols>
   <sheetData>
     <row r="1" s="92" customFormat="1" spans="1:6">
       <c r="A1" s="87" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C1" s="87" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D1" s="87" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E1" s="87" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F1" s="87" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" s="92" customFormat="1" ht="75" spans="1:6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" s="92" customFormat="1" ht="56.25" spans="1:6">
       <c r="A2" s="89">
         <v>501</v>
       </c>
@@ -4162,17 +4317,17 @@
         <v>55</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="D2" s="89"/>
       <c r="E2" s="89" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="93" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" s="92" customFormat="1" ht="112.5" spans="1:6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" s="92" customFormat="1" ht="75" spans="1:6">
       <c r="A3" s="89">
         <v>502</v>
       </c>
@@ -4187,7 +4342,7 @@
         <v>61</v>
       </c>
       <c r="F3" s="93" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4205,6 +4360,54 @@
         <v>66</v>
       </c>
       <c r="F4" s="93"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="89">
+        <v>504</v>
+      </c>
+      <c r="B5" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="93"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="89">
+        <v>505</v>
+      </c>
+      <c r="B6" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="93"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="89">
+        <v>506</v>
+      </c>
+      <c r="B7" s="89" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4219,7 +4422,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -4228,27 +4431,27 @@
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="12.375" customWidth="1"/>
     <col min="4" max="4" width="26.25" customWidth="1"/>
-    <col min="5" max="5" width="64.25" style="86" customWidth="1"/>
+    <col min="5" max="5" width="36.625" style="86" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" spans="1:5">
       <c r="A1" s="87" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C1" s="87" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D1" s="87" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" ht="75" spans="1:5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" ht="93.75" spans="1:5">
       <c r="A2" s="89">
         <v>601</v>
       </c>
@@ -4262,7 +4465,7 @@
         <v>69</v>
       </c>
       <c r="E2" s="90" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" ht="18.75" spans="1:5">
@@ -4300,45 +4503,45 @@
         <v>604</v>
       </c>
       <c r="B5" s="89" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D5" s="89" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E5" s="90"/>
     </row>
-    <row r="6" ht="18.75" spans="1:5">
-      <c r="A6" s="91">
+    <row r="6" ht="56.25" spans="1:5">
+      <c r="A6" s="89">
         <v>605</v>
       </c>
       <c r="B6" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="89" t="s">
-        <v>79</v>
-      </c>
       <c r="D6" s="89" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E6" s="90" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" ht="18.75" spans="1:5">
-      <c r="A7" s="91">
+      <c r="A7" s="89">
         <v>606</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C7" s="89" t="s">
         <v>68</v>
       </c>
       <c r="D7" s="89" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E7" s="90"/>
     </row>
@@ -4347,13 +4550,13 @@
         <v>607</v>
       </c>
       <c r="B8" s="89" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C8" s="89" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="89" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E8" s="90"/>
     </row>
@@ -4362,43 +4565,43 @@
         <v>608</v>
       </c>
       <c r="B9" s="89" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C9" s="89" t="s">
         <v>68</v>
       </c>
       <c r="D9" s="89" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E9" s="90"/>
     </row>
     <row r="10" ht="18.75" spans="1:5">
-      <c r="A10" s="91">
+      <c r="A10" s="89">
         <v>609</v>
       </c>
       <c r="B10" s="89" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C10" s="89" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="89" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="E10" s="90"/>
     </row>
     <row r="11" ht="18.75" spans="1:5">
-      <c r="A11" s="91">
+      <c r="A11" s="89">
         <v>610</v>
       </c>
       <c r="B11" s="89" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C11" s="89" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D11" s="89" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E11" s="90"/>
     </row>
@@ -4411,15 +4614,15 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="21.7666666666667" customWidth="1"/>
     <col min="2" max="2" width="23.35" customWidth="1"/>
@@ -4428,35 +4631,46 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="81" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B1" s="81" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C1" s="82" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" ht="81" spans="1:3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" ht="40.5" spans="1:3">
       <c r="A2" s="83" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="83" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C2" s="84" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="83" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B3" s="85" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C3" s="85" t="s">
-        <v>122</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="83" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4469,12 +4683,12 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -4488,24 +4702,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="77" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B1" s="77" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="77" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="D1" s="77" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="E1" s="77" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A2" s="78" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
@@ -4514,24 +4728,24 @@
     </row>
     <row r="3" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A3" s="79" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="B3" s="79" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E3" s="80" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A4" s="78" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B4" s="79"/>
       <c r="C4" s="79"/>
@@ -4540,24 +4754,24 @@
     </row>
     <row r="5" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A5" s="79" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B5" s="79" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E5" s="80" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A6" s="78" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B6" s="79"/>
       <c r="C6" s="79"/>
@@ -4566,24 +4780,24 @@
     </row>
     <row r="7" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A7" s="79" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B7" s="79" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D7" s="79" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E7" s="80" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A8" s="78" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B8" s="79"/>
       <c r="C8" s="79"/>
@@ -4592,19 +4806,19 @@
     </row>
     <row r="9" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A9" s="79" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B9" s="79" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="79" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E9" s="80" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" s="76" customFormat="1" ht="18.75" spans="1:5">
@@ -4618,75 +4832,75 @@
     </row>
     <row r="11" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A11" s="79" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="C11" s="79" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D11" s="79" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E11" s="80" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A12" s="79" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D12" s="79" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E12" s="80" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A13" s="79" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B13" s="79" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C13" s="79" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D13" s="79" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E13" s="80" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A14" s="79" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B14" s="79" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C14" s="79" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D14" s="79" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E14" s="80" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A15" s="78" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B15" s="79"/>
       <c r="C15" s="79"/>
@@ -4695,75 +4909,75 @@
     </row>
     <row r="16" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A16" s="79" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B16" s="79" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C16" s="79" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D16" s="79" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E16" s="80" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A17" s="79" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="79" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="79" t="s">
+      <c r="D17" s="79" t="s">
         <v>148</v>
       </c>
-      <c r="C17" s="79" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" s="79" t="s">
-        <v>137</v>
-      </c>
       <c r="E17" s="80" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A18" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="79" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="80" t="s">
         <v>149</v>
-      </c>
-      <c r="B18" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="79" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18" s="80" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="19" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A19" s="79" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B19" s="79" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C19" s="79" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D19" s="79" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E19" s="80" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A20" s="78" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="B20" s="79"/>
       <c r="C20" s="79"/>
@@ -4772,130 +4986,156 @@
     </row>
     <row r="21" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A21" s="79" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="B21" s="79" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C21" s="79" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D21" s="79" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E21" s="80" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A22" s="79" t="s">
-        <v>160</v>
-      </c>
-      <c r="B22" s="79" t="s">
-        <v>161</v>
-      </c>
-      <c r="C22" s="79" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="E22" s="80" t="s">
-        <v>132</v>
-      </c>
+      <c r="A22" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="79"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="80"/>
     </row>
     <row r="23" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A23" s="79" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B23" s="79" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C23" s="79" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="D23" s="79" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="E23" s="80" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A24" s="78" t="s">
-        <v>164</v>
-      </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="80"/>
+      <c r="A24" s="79" t="s">
+        <v>174</v>
+      </c>
+      <c r="B24" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="80" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="25" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A25" s="79" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="B25" s="79" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="C25" s="79" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D25" s="79" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E25" s="80" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A26" s="79" t="s">
-        <v>167</v>
-      </c>
-      <c r="B26" s="79" t="s">
-        <v>168</v>
-      </c>
-      <c r="C26" s="79" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="E26" s="80" t="s">
-        <v>138</v>
-      </c>
+      <c r="A26" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" s="79"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="80"/>
     </row>
     <row r="27" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A27" s="79" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B27" s="79" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C27" s="79" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D27" s="79" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="E27" s="80" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" s="76" customFormat="1" ht="18.75" spans="1:5">
       <c r="A28" s="79" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B28" s="79" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C28" s="79" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="D28" s="79" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="E28" s="80" t="s">
-        <v>132</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A29" s="79" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="79" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29" s="80" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" s="76" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A30" s="79" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="79" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" s="80" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -4925,41 +5165,41 @@
   <sheetData>
     <row r="1" ht="21" spans="1:5">
       <c r="A1" s="74" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="B1" s="74" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="C1" s="74" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="E1" s="74" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" ht="21" spans="1:5">
       <c r="A2" s="74" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" ht="21" spans="1:5">
       <c r="A3" s="74" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="B3" s="14">
         <v>5</v>
@@ -4976,44 +5216,44 @@
     </row>
     <row r="4" ht="21" spans="1:6">
       <c r="A4" s="74" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="E4" s="75" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" ht="21" spans="1:5">
       <c r="A5" s="74" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="E5" s="75" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" ht="21" spans="1:5">
       <c r="A6" s="74" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
@@ -5030,22 +5270,22 @@
     </row>
     <row r="7" ht="21" spans="1:5">
       <c r="A7" s="74" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="75" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" ht="21" spans="1:5">
       <c r="A8" s="74" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="B8" s="75">
         <v>0</v>
@@ -5062,7 +5302,7 @@
     </row>
     <row r="9" ht="21" spans="1:5">
       <c r="A9" s="74" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="B9" s="75">
         <v>0</v>
@@ -5105,13 +5345,13 @@
   <sheetData>
     <row r="1" ht="14.25" spans="1:7">
       <c r="A1" s="53" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
@@ -5124,16 +5364,16 @@
       <c r="A2" s="59"/>
       <c r="B2" s="60"/>
       <c r="C2" s="61" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="F2" s="62" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="G2" s="63"/>
     </row>
@@ -5142,23 +5382,23 @@
         <v>4000</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="D3" s="66"/>
       <c r="E3" s="67"/>
       <c r="F3" s="64"/>
       <c r="G3" s="67" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="64"/>
       <c r="B4" s="68"/>
       <c r="C4" s="66" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="D4" s="66"/>
       <c r="E4" s="67"/>
@@ -5170,16 +5410,16 @@
         <v>4001</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="D5" s="66"/>
       <c r="E5" s="67"/>
       <c r="F5" s="64"/>
       <c r="G5" s="67" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5187,23 +5427,23 @@
         <v>4002</v>
       </c>
       <c r="B6" s="70" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="D6" s="66"/>
       <c r="E6" s="67"/>
       <c r="F6" s="64"/>
       <c r="G6" s="69" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="71"/>
       <c r="B7" s="68"/>
       <c r="C7" s="66" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="D7" s="66"/>
       <c r="E7" s="67"/>
@@ -5214,10 +5454,10 @@
       <c r="A8" s="71"/>
       <c r="B8" s="68"/>
       <c r="C8" s="66" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="E8" s="67"/>
       <c r="F8" s="64"/>
@@ -5227,7 +5467,7 @@
       <c r="A9" s="72"/>
       <c r="B9" s="73"/>
       <c r="C9" s="66" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="D9" s="66"/>
       <c r="E9" s="66"/>
@@ -5239,13 +5479,13 @@
         <v>4003</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="E10" s="66"/>
       <c r="F10" s="66"/>
@@ -5255,10 +5495,10 @@
       <c r="A11" s="72"/>
       <c r="B11" s="73"/>
       <c r="C11" s="66" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="D11" s="66" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="E11" s="66"/>
       <c r="F11" s="66"/>
@@ -5269,10 +5509,10 @@
         <v>4004</v>
       </c>
       <c r="B12" s="70" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="D12" s="66"/>
       <c r="E12" s="66"/>
@@ -5283,7 +5523,7 @@
       <c r="A13" s="72"/>
       <c r="B13" s="73"/>
       <c r="C13" s="66" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="D13" s="66"/>
       <c r="E13" s="66"/>
@@ -5295,10 +5535,10 @@
         <v>4005</v>
       </c>
       <c r="B14" s="70" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="C14" s="66" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="D14" s="66"/>
       <c r="E14" s="66"/>
@@ -5309,7 +5549,7 @@
       <c r="A15" s="72"/>
       <c r="B15" s="73"/>
       <c r="C15" s="66" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="D15" s="66"/>
       <c r="E15" s="66"/>
@@ -5321,10 +5561,10 @@
         <v>4006</v>
       </c>
       <c r="B16" s="70" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="C16" s="66" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="D16" s="66"/>
       <c r="E16" s="66"/>
@@ -5335,7 +5575,7 @@
       <c r="A17" s="72"/>
       <c r="B17" s="73"/>
       <c r="C17" s="66" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="D17" s="66"/>
       <c r="E17" s="66"/>
@@ -5347,10 +5587,10 @@
         <v>4007</v>
       </c>
       <c r="B18" s="70" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="C18" s="66" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="D18" s="66"/>
       <c r="E18" s="66"/>
@@ -5361,7 +5601,7 @@
       <c r="A19" s="72"/>
       <c r="B19" s="73"/>
       <c r="C19" s="66" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="D19" s="66"/>
       <c r="E19" s="66"/>
@@ -5373,10 +5613,10 @@
         <v>4008</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="C20" s="66" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="D20" s="66"/>
       <c r="E20" s="67"/>
@@ -5387,7 +5627,7 @@
       <c r="A21" s="72"/>
       <c r="B21" s="73"/>
       <c r="C21" s="66" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="D21" s="66"/>
       <c r="E21" s="67"/>

</xml_diff>